<commit_message>
corrige erro no processo InputToDataBase.xaml
</commit_message>
<xml_diff>
--- a/Data/Cidades.xlsx
+++ b/Data/Cidades.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="368">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="409">
   <x:si>
     <x:t>NOME</x:t>
   </x:si>
@@ -949,16 +949,22 @@
     <x:t>37800-000</x:t>
   </x:si>
   <x:si>
+    <x:t>guaxupeano</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HEBER HAMILTON QUINTELLA</x:t>
+  </x:si>
+  <x:si>
     <x:t>Heliodora</x:t>
   </x:si>
   <x:si>
     <x:t>37484-000</x:t>
   </x:si>
   <x:si>
-    <x:t>guaxupeano</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HEBER HAMILTON QUINTELLA</x:t>
+    <x:t>heliodorense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALEX LEOPOLDINO DE LIMA</x:t>
   </x:si>
   <x:si>
     <x:t>Ibiraci</x:t>
@@ -967,40 +973,70 @@
     <x:t>37990-000</x:t>
   </x:si>
   <x:si>
+    <x:t>ibiraciense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ISMAEL SILVA CÂNDIDO</x:t>
+  </x:si>
+  <x:si>
     <x:t>Ibitiúra de Minas</x:t>
   </x:si>
   <x:si>
     <x:t>37790-000</x:t>
   </x:si>
   <x:si>
+    <x:t>ibitiurense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALEXANDRE DE CASSIO BORGES</x:t>
+  </x:si>
+  <x:si>
     <x:t>Ibituruna</x:t>
   </x:si>
   <x:si>
     <x:t>37223-000</x:t>
   </x:si>
   <x:si>
+    <x:t>ibiturunense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FRANCISCO ANTONIO PEREIRA</x:t>
+  </x:si>
+  <x:si>
     <x:t>Ijaci</x:t>
   </x:si>
   <x:si>
     <x:t>37218-000</x:t>
   </x:si>
   <x:si>
+    <x:t>ijaciense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FABIANO DA SILVA MORETI</x:t>
+  </x:si>
+  <x:si>
     <x:t>Ilicínea</x:t>
   </x:si>
   <x:si>
     <x:t>37175-000</x:t>
   </x:si>
   <x:si>
+    <x:t>ilicineaense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NIRLEI CRISTIANI</x:t>
+  </x:si>
+  <x:si>
     <x:t>Inconfidentes</x:t>
   </x:si>
   <x:si>
     <x:t>37576-000</x:t>
   </x:si>
   <x:si>
-    <x:t>ibitiurense</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ALEXANDRE DE CASSIO BORGES</x:t>
+    <x:t>inconfidentino</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ROSÂNGELA MARIA DANTAS</x:t>
   </x:si>
   <x:si>
     <x:t>Ingaí</x:t>
@@ -1009,22 +1045,34 @@
     <x:t>37215-000</x:t>
   </x:si>
   <x:si>
+    <x:t>ingaiense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GIULLIANO RIBEIRO PINTO</x:t>
+  </x:si>
+  <x:si>
     <x:t>Ipuiúna</x:t>
   </x:si>
   <x:si>
     <x:t>37588-000</x:t>
   </x:si>
   <x:si>
+    <x:t>ipuiunense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ELDER CASSIO DE SOUZA OLIVA</x:t>
+  </x:si>
+  <x:si>
     <x:t>Itajubá</x:t>
   </x:si>
   <x:si>
     <x:t>37500-001</x:t>
   </x:si>
   <x:si>
-    <x:t>ijaciense</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FABIANO DA SILVA MORETI</x:t>
+    <x:t>Itajubense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CHRISTIAN GONÇALVES TIBURZIO E SILVA</x:t>
   </x:si>
   <x:si>
     <x:t>Itamogi</x:t>
@@ -1033,16 +1081,22 @@
     <x:t>37973-000</x:t>
   </x:si>
   <x:si>
+    <x:t>itamogiense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RONALDO PEREIRA DIAS</x:t>
+  </x:si>
+  <x:si>
     <x:t>Itamonte</x:t>
   </x:si>
   <x:si>
     <x:t>37466-000</x:t>
   </x:si>
   <x:si>
-    <x:t>ibiturunense</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GIULLIANO RIBEIRO PINTO</x:t>
+    <x:t>itamontense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ALEXANDRE AUGUSTO MOREIRA SANTOS</x:t>
   </x:si>
   <x:si>
     <x:t>Itanhandu</x:t>
@@ -1051,7 +1105,10 @@
     <x:t>37464-000</x:t>
   </x:si>
   <x:si>
-    <x:t>ingaiense</x:t>
+    <x:t>itanhanduense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CARLOS GONÇALVES DA FONSECA</x:t>
   </x:si>
   <x:si>
     <x:t>Itapeva</x:t>
@@ -1060,64 +1117,130 @@
     <x:t>37655-000</x:t>
   </x:si>
   <x:si>
+    <x:t>itapevense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DANIEL PEREIRA DO COUTO</x:t>
+  </x:si>
+  <x:si>
     <x:t>Itaú de Minas</x:t>
   </x:si>
   <x:si>
     <x:t>37975-000</x:t>
   </x:si>
   <x:si>
+    <x:t>itauense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NORIVAL FRANCISCO DE LIMA</x:t>
+  </x:si>
+  <x:si>
     <x:t>Itumirim</x:t>
   </x:si>
   <x:si>
     <x:t>37210-000</x:t>
   </x:si>
   <x:si>
+    <x:t>itumirinense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CARLOS ALBERTO NASCIMENTO</x:t>
+  </x:si>
+  <x:si>
     <x:t>Jacutinga</x:t>
   </x:si>
   <x:si>
     <x:t>37590-000</x:t>
   </x:si>
   <x:si>
+    <x:t>jacutinguense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MELQUIADES DE ARAUJO</x:t>
+  </x:si>
+  <x:si>
     <x:t>Jacuí</x:t>
   </x:si>
   <x:si>
     <x:t>37965-000</x:t>
   </x:si>
   <x:si>
+    <x:t>jacuiense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MARIA CONCEICAO DOS REIS PEREIRA</x:t>
+  </x:si>
+  <x:si>
     <x:t>Jesuânia</x:t>
   </x:si>
   <x:si>
     <x:t>37485-000</x:t>
   </x:si>
   <x:si>
+    <x:t>jesuanense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JOSÉ LAÉRCIO BRANDÃO DE CASTRO</x:t>
+  </x:si>
+  <x:si>
     <x:t>Juruaia</x:t>
   </x:si>
   <x:si>
     <x:t>37805-000</x:t>
   </x:si>
   <x:si>
+    <x:t>juruaiense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ÁLVARO MARIANO JÚNIOR</x:t>
+  </x:si>
+  <x:si>
     <x:t>Lambari</x:t>
   </x:si>
   <x:si>
     <x:t>37480-000</x:t>
   </x:si>
   <x:si>
+    <x:t>lambariense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MARCELO GIOVANI DE SOUSA</x:t>
+  </x:si>
+  <x:si>
     <x:t>Lavras</x:t>
   </x:si>
   <x:si>
     <x:t>37200-001</x:t>
   </x:si>
   <x:si>
+    <x:t>lavrense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JUSSARA MENICUCCI DE OLIVEIRA</x:t>
+  </x:si>
+  <x:si>
     <x:t>Liberdade</x:t>
   </x:si>
   <x:si>
     <x:t>37350-000</x:t>
   </x:si>
   <x:si>
+    <x:t>libertense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WALTER DE ASSIS TOLEDO JUNIOR</x:t>
+  </x:si>
+  <x:si>
     <x:t>Luminárias</x:t>
   </x:si>
   <x:si>
     <x:t>37240-000</x:t>
+  </x:si>
+  <x:si>
+    <x:t>luminarense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ECIO CARVALHO REZENDE</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -3599,7 +3722,7 @@
         <x:v>298</x:v>
       </x:c>
       <x:c r="C74" s="0" t="n">
-        <x:v>4437</x:v>
+        <x:v>4355</x:v>
       </x:c>
       <x:c r="D74" s="0" t="n">
         <x:v>4220</x:v>
@@ -3686,225 +3809,225 @@
         <x:v>310</x:v>
       </x:c>
       <x:c r="C77" s="0" t="n">
-        <x:v>19017</x:v>
+        <x:v>52078</x:v>
       </x:c>
       <x:c r="D77" s="0" t="n">
-        <x:v>18714</x:v>
+        <x:v>49430</x:v>
       </x:c>
       <x:c r="E77" s="0" t="n">
-        <x:v>63.47</x:v>
+        <x:v>172.59</x:v>
       </x:c>
       <x:c r="F77" s="0" t="n">
-        <x:v>3128303</x:v>
+        <x:v>3128709</x:v>
       </x:c>
       <x:c r="G77" s="0" t="s">
-        <x:v>307</x:v>
+        <x:v>311</x:v>
       </x:c>
       <x:c r="H77" s="0" t="s">
-        <x:v>308</x:v>
+        <x:v>312</x:v>
       </x:c>
       <x:c r="I77" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="78" spans="1:9">
       <x:c r="A78" s="0" t="s">
-        <x:v>311</x:v>
+        <x:v>313</x:v>
       </x:c>
       <x:c r="B78" s="0" t="s">
-        <x:v>312</x:v>
+        <x:v>314</x:v>
       </x:c>
       <x:c r="C78" s="0" t="n">
-        <x:v>52078</x:v>
+        <x:v>6591</x:v>
       </x:c>
       <x:c r="D78" s="0" t="n">
-        <x:v>49430</x:v>
+        <x:v>6121</x:v>
       </x:c>
       <x:c r="E78" s="0" t="n">
-        <x:v>172.59</x:v>
+        <x:v>39.76</x:v>
       </x:c>
       <x:c r="F78" s="0" t="n">
-        <x:v>3128709</x:v>
+        <x:v>3129202</x:v>
       </x:c>
       <x:c r="G78" s="0" t="s">
-        <x:v>313</x:v>
+        <x:v>315</x:v>
       </x:c>
       <x:c r="H78" s="0" t="s">
-        <x:v>314</x:v>
+        <x:v>316</x:v>
       </x:c>
       <x:c r="I78" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="79" spans="1:9">
       <x:c r="A79" s="0" t="s">
-        <x:v>315</x:v>
+        <x:v>317</x:v>
       </x:c>
       <x:c r="B79" s="0" t="s">
-        <x:v>316</x:v>
+        <x:v>318</x:v>
       </x:c>
       <x:c r="C79" s="0" t="n">
-        <x:v>52078</x:v>
+        <x:v>13986</x:v>
       </x:c>
       <x:c r="D79" s="0" t="n">
-        <x:v>49430</x:v>
+        <x:v>12176</x:v>
       </x:c>
       <x:c r="E79" s="0" t="n">
-        <x:v>172.59</x:v>
+        <x:v>21.66</x:v>
       </x:c>
       <x:c r="F79" s="0" t="n">
-        <x:v>3128709</x:v>
+        <x:v>3129707</x:v>
       </x:c>
       <x:c r="G79" s="0" t="s">
-        <x:v>313</x:v>
+        <x:v>319</x:v>
       </x:c>
       <x:c r="H79" s="0" t="s">
-        <x:v>314</x:v>
+        <x:v>320</x:v>
       </x:c>
       <x:c r="I79" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="80" spans="1:9">
       <x:c r="A80" s="0" t="s">
-        <x:v>317</x:v>
+        <x:v>321</x:v>
       </x:c>
       <x:c r="B80" s="0" t="s">
-        <x:v>318</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="C80" s="0" t="n">
-        <x:v>52078</x:v>
+        <x:v>3492</x:v>
       </x:c>
       <x:c r="D80" s="0" t="n">
-        <x:v>49430</x:v>
+        <x:v>3382</x:v>
       </x:c>
       <x:c r="E80" s="0" t="n">
-        <x:v>172.59</x:v>
+        <x:v>49.51</x:v>
       </x:c>
       <x:c r="F80" s="0" t="n">
-        <x:v>3128709</x:v>
+        <x:v>3129905</x:v>
       </x:c>
       <x:c r="G80" s="0" t="s">
-        <x:v>313</x:v>
+        <x:v>323</x:v>
       </x:c>
       <x:c r="H80" s="0" t="s">
-        <x:v>314</x:v>
+        <x:v>324</x:v>
       </x:c>
       <x:c r="I80" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="81" spans="1:9">
       <x:c r="A81" s="0" t="s">
-        <x:v>319</x:v>
+        <x:v>325</x:v>
       </x:c>
       <x:c r="B81" s="0" t="s">
-        <x:v>320</x:v>
+        <x:v>326</x:v>
       </x:c>
       <x:c r="C81" s="0" t="n">
-        <x:v>52078</x:v>
+        <x:v>2996</x:v>
       </x:c>
       <x:c r="D81" s="0" t="n">
-        <x:v>49430</x:v>
+        <x:v>2866</x:v>
       </x:c>
       <x:c r="E81" s="0" t="n">
-        <x:v>172.59</x:v>
+        <x:v>18.72</x:v>
       </x:c>
       <x:c r="F81" s="0" t="n">
-        <x:v>3128709</x:v>
+        <x:v>3130002</x:v>
       </x:c>
       <x:c r="G81" s="0" t="s">
-        <x:v>313</x:v>
+        <x:v>327</x:v>
       </x:c>
       <x:c r="H81" s="0" t="s">
-        <x:v>314</x:v>
+        <x:v>328</x:v>
       </x:c>
       <x:c r="I81" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="82" spans="1:9">
       <x:c r="A82" s="0" t="s">
-        <x:v>321</x:v>
+        <x:v>329</x:v>
       </x:c>
       <x:c r="B82" s="0" t="s">
-        <x:v>322</x:v>
+        <x:v>330</x:v>
       </x:c>
       <x:c r="C82" s="0" t="n">
-        <x:v>52078</x:v>
+        <x:v>6610</x:v>
       </x:c>
       <x:c r="D82" s="0" t="n">
-        <x:v>49430</x:v>
+        <x:v>5859</x:v>
       </x:c>
       <x:c r="E82" s="0" t="n">
-        <x:v>172.59</x:v>
+        <x:v>55.67</x:v>
       </x:c>
       <x:c r="F82" s="0" t="n">
-        <x:v>3128709</x:v>
+        <x:v>3130408</x:v>
       </x:c>
       <x:c r="G82" s="0" t="s">
-        <x:v>313</x:v>
+        <x:v>331</x:v>
       </x:c>
       <x:c r="H82" s="0" t="s">
-        <x:v>314</x:v>
+        <x:v>332</x:v>
       </x:c>
       <x:c r="I82" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="83" spans="1:9">
       <x:c r="A83" s="0" t="s">
-        <x:v>323</x:v>
+        <x:v>333</x:v>
       </x:c>
       <x:c r="B83" s="0" t="s">
-        <x:v>324</x:v>
+        <x:v>334</x:v>
       </x:c>
       <x:c r="C83" s="0" t="n">
-        <x:v>52078</x:v>
+        <x:v>12444</x:v>
       </x:c>
       <x:c r="D83" s="0" t="n">
-        <x:v>49430</x:v>
+        <x:v>11488</x:v>
       </x:c>
       <x:c r="E83" s="0" t="n">
-        <x:v>172.59</x:v>
+        <x:v>30.53</x:v>
       </x:c>
       <x:c r="F83" s="0" t="n">
-        <x:v>3128709</x:v>
+        <x:v>3130507</x:v>
       </x:c>
       <x:c r="G83" s="0" t="s">
-        <x:v>313</x:v>
+        <x:v>335</x:v>
       </x:c>
       <x:c r="H83" s="0" t="s">
-        <x:v>314</x:v>
+        <x:v>336</x:v>
       </x:c>
       <x:c r="I83" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="84" spans="1:9">
       <x:c r="A84" s="0" t="s">
-        <x:v>325</x:v>
+        <x:v>337</x:v>
       </x:c>
       <x:c r="B84" s="0" t="s">
-        <x:v>326</x:v>
+        <x:v>338</x:v>
       </x:c>
       <x:c r="C84" s="0" t="n">
-        <x:v>3492</x:v>
+        <x:v>7358</x:v>
       </x:c>
       <x:c r="D84" s="0" t="n">
-        <x:v>3382</x:v>
+        <x:v>6908</x:v>
       </x:c>
       <x:c r="E84" s="0" t="n">
-        <x:v>49.51</x:v>
+        <x:v>46.17</x:v>
       </x:c>
       <x:c r="F84" s="0" t="n">
-        <x:v>3129905</x:v>
+        <x:v>3130606</x:v>
       </x:c>
       <x:c r="G84" s="0" t="s">
-        <x:v>327</x:v>
+        <x:v>339</x:v>
       </x:c>
       <x:c r="H84" s="0" t="s">
-        <x:v>328</x:v>
+        <x:v>340</x:v>
       </x:c>
       <x:c r="I84" s="0" t="n">
         <x:v>1</x:v>
@@ -3912,28 +4035,28 @@
     </x:row>
     <x:row r="85" spans="1:9">
       <x:c r="A85" s="0" t="s">
-        <x:v>329</x:v>
+        <x:v>341</x:v>
       </x:c>
       <x:c r="B85" s="0" t="s">
-        <x:v>330</x:v>
+        <x:v>342</x:v>
       </x:c>
       <x:c r="C85" s="0" t="n">
-        <x:v>3492</x:v>
+        <x:v>2776</x:v>
       </x:c>
       <x:c r="D85" s="0" t="n">
-        <x:v>3382</x:v>
+        <x:v>2629</x:v>
       </x:c>
       <x:c r="E85" s="0" t="n">
-        <x:v>49.51</x:v>
+        <x:v>8.6</x:v>
       </x:c>
       <x:c r="F85" s="0" t="n">
-        <x:v>3129905</x:v>
+        <x:v>3130804</x:v>
       </x:c>
       <x:c r="G85" s="0" t="s">
-        <x:v>327</x:v>
+        <x:v>343</x:v>
       </x:c>
       <x:c r="H85" s="0" t="s">
-        <x:v>328</x:v>
+        <x:v>344</x:v>
       </x:c>
       <x:c r="I85" s="0" t="n">
         <x:v>1</x:v>
@@ -3941,28 +4064,28 @@
     </x:row>
     <x:row r="86" spans="1:9">
       <x:c r="A86" s="0" t="s">
-        <x:v>331</x:v>
+        <x:v>345</x:v>
       </x:c>
       <x:c r="B86" s="0" t="s">
-        <x:v>332</x:v>
+        <x:v>346</x:v>
       </x:c>
       <x:c r="C86" s="0" t="n">
-        <x:v>3492</x:v>
+        <x:v>10118</x:v>
       </x:c>
       <x:c r="D86" s="0" t="n">
-        <x:v>3382</x:v>
+        <x:v>9521</x:v>
       </x:c>
       <x:c r="E86" s="0" t="n">
-        <x:v>49.51</x:v>
+        <x:v>31.93</x:v>
       </x:c>
       <x:c r="F86" s="0" t="n">
-        <x:v>3129905</x:v>
+        <x:v>3131505</x:v>
       </x:c>
       <x:c r="G86" s="0" t="s">
-        <x:v>327</x:v>
+        <x:v>347</x:v>
       </x:c>
       <x:c r="H86" s="0" t="s">
-        <x:v>328</x:v>
+        <x:v>348</x:v>
       </x:c>
       <x:c r="I86" s="0" t="n">
         <x:v>1</x:v>
@@ -3970,57 +4093,57 @@
     </x:row>
     <x:row r="87" spans="1:9">
       <x:c r="A87" s="0" t="s">
-        <x:v>333</x:v>
+        <x:v>349</x:v>
       </x:c>
       <x:c r="B87" s="0" t="s">
-        <x:v>334</x:v>
+        <x:v>350</x:v>
       </x:c>
       <x:c r="C87" s="0" t="n">
-        <x:v>6610</x:v>
+        <x:v>97334</x:v>
       </x:c>
       <x:c r="D87" s="0" t="n">
-        <x:v>5859</x:v>
+        <x:v>90658</x:v>
       </x:c>
       <x:c r="E87" s="0" t="n">
-        <x:v>55.67</x:v>
+        <x:v>307.49</x:v>
       </x:c>
       <x:c r="F87" s="0" t="n">
-        <x:v>3130408</x:v>
+        <x:v>3132404</x:v>
       </x:c>
       <x:c r="G87" s="0" t="s">
-        <x:v>335</x:v>
+        <x:v>351</x:v>
       </x:c>
       <x:c r="H87" s="0" t="s">
-        <x:v>336</x:v>
+        <x:v>352</x:v>
       </x:c>
       <x:c r="I87" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="88" spans="1:9">
       <x:c r="A88" s="0" t="s">
-        <x:v>337</x:v>
+        <x:v>353</x:v>
       </x:c>
       <x:c r="B88" s="0" t="s">
-        <x:v>338</x:v>
+        <x:v>354</x:v>
       </x:c>
       <x:c r="C88" s="0" t="n">
-        <x:v>6610</x:v>
+        <x:v>10157</x:v>
       </x:c>
       <x:c r="D88" s="0" t="n">
-        <x:v>5859</x:v>
+        <x:v>10349</x:v>
       </x:c>
       <x:c r="E88" s="0" t="n">
-        <x:v>55.67</x:v>
+        <x:v>42.47</x:v>
       </x:c>
       <x:c r="F88" s="0" t="n">
-        <x:v>3130408</x:v>
+        <x:v>3132909</x:v>
       </x:c>
       <x:c r="G88" s="0" t="s">
-        <x:v>335</x:v>
+        <x:v>355</x:v>
       </x:c>
       <x:c r="H88" s="0" t="s">
-        <x:v>336</x:v>
+        <x:v>356</x:v>
       </x:c>
       <x:c r="I88" s="0" t="n">
         <x:v>1</x:v>
@@ -4028,86 +4151,86 @@
     </x:row>
     <x:row r="89" spans="1:9">
       <x:c r="A89" s="0" t="s">
-        <x:v>339</x:v>
+        <x:v>357</x:v>
       </x:c>
       <x:c r="B89" s="0" t="s">
-        <x:v>340</x:v>
+        <x:v>358</x:v>
       </x:c>
       <x:c r="C89" s="0" t="n">
-        <x:v>6610</x:v>
+        <x:v>15714</x:v>
       </x:c>
       <x:c r="D89" s="0" t="n">
-        <x:v>5859</x:v>
+        <x:v>14003</x:v>
       </x:c>
       <x:c r="E89" s="0" t="n">
-        <x:v>55.67</x:v>
+        <x:v>32.43</x:v>
       </x:c>
       <x:c r="F89" s="0" t="n">
-        <x:v>3130606</x:v>
+        <x:v>3133006</x:v>
       </x:c>
       <x:c r="G89" s="0" t="s">
-        <x:v>341</x:v>
+        <x:v>359</x:v>
       </x:c>
       <x:c r="H89" s="0" t="s">
-        <x:v>342</x:v>
+        <x:v>360</x:v>
       </x:c>
       <x:c r="I89" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="90" spans="1:9">
       <x:c r="A90" s="0" t="s">
-        <x:v>343</x:v>
+        <x:v>361</x:v>
       </x:c>
       <x:c r="B90" s="0" t="s">
-        <x:v>344</x:v>
+        <x:v>362</x:v>
       </x:c>
       <x:c r="C90" s="0" t="n">
-        <x:v>2776</x:v>
+        <x:v>15423</x:v>
       </x:c>
       <x:c r="D90" s="0" t="n">
-        <x:v>2629</x:v>
+        <x:v>14175</x:v>
       </x:c>
       <x:c r="E90" s="0" t="n">
-        <x:v>8.6</x:v>
+        <x:v>98.87</x:v>
       </x:c>
       <x:c r="F90" s="0" t="n">
-        <x:v>3130804</x:v>
+        <x:v>3133105</x:v>
       </x:c>
       <x:c r="G90" s="0" t="s">
-        <x:v>345</x:v>
+        <x:v>363</x:v>
       </x:c>
       <x:c r="H90" s="0" t="s">
-        <x:v>342</x:v>
+        <x:v>364</x:v>
       </x:c>
       <x:c r="I90" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="91" spans="1:9">
       <x:c r="A91" s="0" t="s">
-        <x:v>346</x:v>
+        <x:v>365</x:v>
       </x:c>
       <x:c r="B91" s="0" t="s">
-        <x:v>347</x:v>
+        <x:v>366</x:v>
       </x:c>
       <x:c r="C91" s="0" t="n">
-        <x:v>2776</x:v>
+        <x:v>9881</x:v>
       </x:c>
       <x:c r="D91" s="0" t="n">
-        <x:v>2629</x:v>
+        <x:v>8664</x:v>
       </x:c>
       <x:c r="E91" s="0" t="n">
-        <x:v>8.6</x:v>
+        <x:v>48.85</x:v>
       </x:c>
       <x:c r="F91" s="0" t="n">
-        <x:v>3130804</x:v>
+        <x:v>3133600</x:v>
       </x:c>
       <x:c r="G91" s="0" t="s">
-        <x:v>345</x:v>
+        <x:v>367</x:v>
       </x:c>
       <x:c r="H91" s="0" t="s">
-        <x:v>342</x:v>
+        <x:v>368</x:v>
       </x:c>
       <x:c r="I91" s="0" t="n">
         <x:v>1</x:v>
@@ -4115,57 +4238,57 @@
     </x:row>
     <x:row r="92" spans="1:9">
       <x:c r="A92" s="0" t="s">
-        <x:v>348</x:v>
+        <x:v>369</x:v>
       </x:c>
       <x:c r="B92" s="0" t="s">
-        <x:v>349</x:v>
+        <x:v>370</x:v>
       </x:c>
       <x:c r="C92" s="0" t="n">
-        <x:v>2776</x:v>
+        <x:v>16199</x:v>
       </x:c>
       <x:c r="D92" s="0" t="n">
-        <x:v>2629</x:v>
+        <x:v>14945</x:v>
       </x:c>
       <x:c r="E92" s="0" t="n">
-        <x:v>8.6</x:v>
+        <x:v>97.41</x:v>
       </x:c>
       <x:c r="F92" s="0" t="n">
-        <x:v>3130804</x:v>
+        <x:v>3133758</x:v>
       </x:c>
       <x:c r="G92" s="0" t="s">
-        <x:v>345</x:v>
+        <x:v>371</x:v>
       </x:c>
       <x:c r="H92" s="0" t="s">
-        <x:v>342</x:v>
+        <x:v>372</x:v>
       </x:c>
       <x:c r="I92" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="93" spans="1:9">
       <x:c r="A93" s="0" t="s">
-        <x:v>350</x:v>
+        <x:v>373</x:v>
       </x:c>
       <x:c r="B93" s="0" t="s">
-        <x:v>351</x:v>
+        <x:v>374</x:v>
       </x:c>
       <x:c r="C93" s="0" t="n">
-        <x:v>2776</x:v>
+        <x:v>6000</x:v>
       </x:c>
       <x:c r="D93" s="0" t="n">
-        <x:v>2629</x:v>
+        <x:v>6139</x:v>
       </x:c>
       <x:c r="E93" s="0" t="n">
-        <x:v>8.6</x:v>
+        <x:v>26.15</x:v>
       </x:c>
       <x:c r="F93" s="0" t="n">
-        <x:v>3130804</x:v>
+        <x:v>3134301</x:v>
       </x:c>
       <x:c r="G93" s="0" t="s">
-        <x:v>345</x:v>
+        <x:v>375</x:v>
       </x:c>
       <x:c r="H93" s="0" t="s">
-        <x:v>342</x:v>
+        <x:v>376</x:v>
       </x:c>
       <x:c r="I93" s="0" t="n">
         <x:v>1</x:v>
@@ -4173,57 +4296,57 @@
     </x:row>
     <x:row r="94" spans="1:9">
       <x:c r="A94" s="0" t="s">
-        <x:v>352</x:v>
+        <x:v>377</x:v>
       </x:c>
       <x:c r="B94" s="0" t="s">
-        <x:v>353</x:v>
+        <x:v>378</x:v>
       </x:c>
       <x:c r="C94" s="0" t="n">
-        <x:v>2776</x:v>
+        <x:v>26264</x:v>
       </x:c>
       <x:c r="D94" s="0" t="n">
-        <x:v>2629</x:v>
+        <x:v>22772</x:v>
       </x:c>
       <x:c r="E94" s="0" t="n">
-        <x:v>8.6</x:v>
+        <x:v>65.48</x:v>
       </x:c>
       <x:c r="F94" s="0" t="n">
-        <x:v>3130804</x:v>
+        <x:v>3134905</x:v>
       </x:c>
       <x:c r="G94" s="0" t="s">
-        <x:v>345</x:v>
+        <x:v>379</x:v>
       </x:c>
       <x:c r="H94" s="0" t="s">
-        <x:v>342</x:v>
+        <x:v>380</x:v>
       </x:c>
       <x:c r="I94" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="95" spans="1:9">
       <x:c r="A95" s="0" t="s">
-        <x:v>354</x:v>
+        <x:v>381</x:v>
       </x:c>
       <x:c r="B95" s="0" t="s">
-        <x:v>355</x:v>
+        <x:v>382</x:v>
       </x:c>
       <x:c r="C95" s="0" t="n">
-        <x:v>2776</x:v>
+        <x:v>7691</x:v>
       </x:c>
       <x:c r="D95" s="0" t="n">
-        <x:v>2629</x:v>
+        <x:v>7502</x:v>
       </x:c>
       <x:c r="E95" s="0" t="n">
-        <x:v>8.6</x:v>
+        <x:v>18.33</x:v>
       </x:c>
       <x:c r="F95" s="0" t="n">
-        <x:v>3130804</x:v>
+        <x:v>3134806</x:v>
       </x:c>
       <x:c r="G95" s="0" t="s">
-        <x:v>345</x:v>
+        <x:v>383</x:v>
       </x:c>
       <x:c r="H95" s="0" t="s">
-        <x:v>342</x:v>
+        <x:v>384</x:v>
       </x:c>
       <x:c r="I95" s="0" t="n">
         <x:v>1</x:v>
@@ -4231,28 +4354,28 @@
     </x:row>
     <x:row r="96" spans="1:9">
       <x:c r="A96" s="0" t="s">
-        <x:v>356</x:v>
+        <x:v>385</x:v>
       </x:c>
       <x:c r="B96" s="0" t="s">
-        <x:v>357</x:v>
+        <x:v>386</x:v>
       </x:c>
       <x:c r="C96" s="0" t="n">
-        <x:v>2776</x:v>
+        <x:v>4780</x:v>
       </x:c>
       <x:c r="D96" s="0" t="n">
-        <x:v>2629</x:v>
+        <x:v>4768</x:v>
       </x:c>
       <x:c r="E96" s="0" t="n">
-        <x:v>8.6</x:v>
+        <x:v>30.99</x:v>
       </x:c>
       <x:c r="F96" s="0" t="n">
-        <x:v>3130804</x:v>
+        <x:v>3135902</x:v>
       </x:c>
       <x:c r="G96" s="0" t="s">
-        <x:v>345</x:v>
+        <x:v>387</x:v>
       </x:c>
       <x:c r="H96" s="0" t="s">
-        <x:v>342</x:v>
+        <x:v>388</x:v>
       </x:c>
       <x:c r="I96" s="0" t="n">
         <x:v>1</x:v>
@@ -4260,28 +4383,28 @@
     </x:row>
     <x:row r="97" spans="1:9">
       <x:c r="A97" s="0" t="s">
-        <x:v>358</x:v>
+        <x:v>389</x:v>
       </x:c>
       <x:c r="B97" s="0" t="s">
-        <x:v>359</x:v>
+        <x:v>390</x:v>
       </x:c>
       <x:c r="C97" s="0" t="n">
-        <x:v>2776</x:v>
+        <x:v>10681</x:v>
       </x:c>
       <x:c r="D97" s="0" t="n">
-        <x:v>2629</x:v>
+        <x:v>9238</x:v>
       </x:c>
       <x:c r="E97" s="0" t="n">
-        <x:v>8.6</x:v>
+        <x:v>41.92</x:v>
       </x:c>
       <x:c r="F97" s="0" t="n">
-        <x:v>3130804</x:v>
+        <x:v>3136900</x:v>
       </x:c>
       <x:c r="G97" s="0" t="s">
-        <x:v>345</x:v>
+        <x:v>391</x:v>
       </x:c>
       <x:c r="H97" s="0" t="s">
-        <x:v>342</x:v>
+        <x:v>392</x:v>
       </x:c>
       <x:c r="I97" s="0" t="n">
         <x:v>1</x:v>
@@ -4289,86 +4412,86 @@
     </x:row>
     <x:row r="98" spans="1:9">
       <x:c r="A98" s="0" t="s">
-        <x:v>360</x:v>
+        <x:v>393</x:v>
       </x:c>
       <x:c r="B98" s="0" t="s">
-        <x:v>361</x:v>
+        <x:v>394</x:v>
       </x:c>
       <x:c r="C98" s="0" t="n">
-        <x:v>2776</x:v>
+        <x:v>20907</x:v>
       </x:c>
       <x:c r="D98" s="0" t="n">
-        <x:v>2629</x:v>
+        <x:v>19554</x:v>
       </x:c>
       <x:c r="E98" s="0" t="n">
-        <x:v>8.6</x:v>
+        <x:v>91.76</x:v>
       </x:c>
       <x:c r="F98" s="0" t="n">
-        <x:v>3130804</x:v>
+        <x:v>3137809</x:v>
       </x:c>
       <x:c r="G98" s="0" t="s">
-        <x:v>345</x:v>
+        <x:v>395</x:v>
       </x:c>
       <x:c r="H98" s="0" t="s">
-        <x:v>342</x:v>
+        <x:v>396</x:v>
       </x:c>
       <x:c r="I98" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="99" spans="1:9">
       <x:c r="A99" s="0" t="s">
-        <x:v>362</x:v>
+        <x:v>397</x:v>
       </x:c>
       <x:c r="B99" s="0" t="s">
-        <x:v>363</x:v>
+        <x:v>398</x:v>
       </x:c>
       <x:c r="C99" s="0" t="n">
-        <x:v>2776</x:v>
+        <x:v>104783</x:v>
       </x:c>
       <x:c r="D99" s="0" t="n">
-        <x:v>2629</x:v>
+        <x:v>92200</x:v>
       </x:c>
       <x:c r="E99" s="0" t="n">
-        <x:v>8.6</x:v>
+        <x:v>163.26</x:v>
       </x:c>
       <x:c r="F99" s="0" t="n">
-        <x:v>3130804</x:v>
+        <x:v>3138203</x:v>
       </x:c>
       <x:c r="G99" s="0" t="s">
-        <x:v>345</x:v>
+        <x:v>399</x:v>
       </x:c>
       <x:c r="H99" s="0" t="s">
-        <x:v>342</x:v>
+        <x:v>400</x:v>
       </x:c>
       <x:c r="I99" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="100" spans="1:9">
       <x:c r="A100" s="0" t="s">
-        <x:v>364</x:v>
+        <x:v>401</x:v>
       </x:c>
       <x:c r="B100" s="0" t="s">
-        <x:v>365</x:v>
+        <x:v>402</x:v>
       </x:c>
       <x:c r="C100" s="0" t="n">
-        <x:v>2776</x:v>
+        <x:v>5031</x:v>
       </x:c>
       <x:c r="D100" s="0" t="n">
-        <x:v>2629</x:v>
+        <x:v>5346</x:v>
       </x:c>
       <x:c r="E100" s="0" t="n">
-        <x:v>8.6</x:v>
+        <x:v>13.32</x:v>
       </x:c>
       <x:c r="F100" s="0" t="n">
-        <x:v>3130804</x:v>
+        <x:v>3138500</x:v>
       </x:c>
       <x:c r="G100" s="0" t="s">
-        <x:v>345</x:v>
+        <x:v>403</x:v>
       </x:c>
       <x:c r="H100" s="0" t="s">
-        <x:v>342</x:v>
+        <x:v>404</x:v>
       </x:c>
       <x:c r="I100" s="0" t="n">
         <x:v>1</x:v>
@@ -4376,28 +4499,28 @@
     </x:row>
     <x:row r="101" spans="1:9">
       <x:c r="A101" s="0" t="s">
-        <x:v>366</x:v>
+        <x:v>405</x:v>
       </x:c>
       <x:c r="B101" s="0" t="s">
-        <x:v>367</x:v>
+        <x:v>406</x:v>
       </x:c>
       <x:c r="C101" s="0" t="n">
-        <x:v>2776</x:v>
+        <x:v>5438</x:v>
       </x:c>
       <x:c r="D101" s="0" t="n">
-        <x:v>2629</x:v>
+        <x:v>5422</x:v>
       </x:c>
       <x:c r="E101" s="0" t="n">
-        <x:v>8.6</x:v>
+        <x:v>10.84</x:v>
       </x:c>
       <x:c r="F101" s="0" t="n">
-        <x:v>3130804</x:v>
+        <x:v>3138708</x:v>
       </x:c>
       <x:c r="G101" s="0" t="s">
-        <x:v>345</x:v>
+        <x:v>407</x:v>
       </x:c>
       <x:c r="H101" s="0" t="s">
-        <x:v>342</x:v>
+        <x:v>408</x:v>
       </x:c>
       <x:c r="I101" s="0" t="n">
         <x:v>1</x:v>

</xml_diff>